<commit_message>
My test Cases Added
</commit_message>
<xml_diff>
--- a/group1/datasets/ronansTestDataset.xlsx
+++ b/group1/datasets/ronansTestDataset.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="3" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Base Data" sheetId="1" state="visible" r:id="rId2"/>
@@ -723,8 +723,8 @@
   </sheetPr>
   <dimension ref="A1:N1001"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="B4" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="K10" activeCellId="1" pane="topLeft" sqref="D16:I173 K10"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="H1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="K6" activeCellId="0" pane="topLeft" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <cols>
@@ -994,9 +994,6 @@
       </c>
       <c r="J6" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="K6" s="2" t="n">
-        <v>344930000000011</v>
       </c>
       <c r="L6" s="2" t="n">
         <v>4.80953208161499E+018</v>
@@ -2411,7 +2408,7 @@
   <dimension ref="A1:C81"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="D16:I173 A1"/>
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <cols>
@@ -3333,7 +3330,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A3" activeCellId="1" pane="topLeft" sqref="D16:I173 A3"/>
+      <selection activeCell="A3" activeCellId="0" pane="topLeft" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <cols>
@@ -3409,8 +3406,8 @@
   </sheetPr>
   <dimension ref="A1:I100"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A13" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="D16" activeCellId="0" pane="topLeft" sqref="D16:I173"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A13" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="D16" activeCellId="0" pane="topLeft" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <cols>
@@ -3965,7 +3962,7 @@
   <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A31" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="D26" activeCellId="0" pane="topLeft" sqref="D16:I173"/>
+      <selection activeCell="D26" activeCellId="0" pane="topLeft" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <cols>

</xml_diff>